<commit_message>
Fixed a typo on the excel example
</commit_message>
<xml_diff>
--- a/Gainsight_Log.xlsx
+++ b/Gainsight_Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicente\Github\GainsightAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicente\Github\gainsight-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD0A08-EF33-45CD-90D1-5D7B38BC03CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737134BC-5403-4475-93BE-6484D85B8E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheets" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <t>You can leave empty columns. Rows will be skipped in case of missing data</t>
   </si>
   <si>
-    <t>You can check the output on the console for the roles that were added</t>
+    <t>You can check the output on the console for the rows that were added</t>
   </si>
 </sst>
 </file>

</xml_diff>